<commit_message>
added the train data
</commit_message>
<xml_diff>
--- a/Frequent Phrases.xlsx
+++ b/Frequent Phrases.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Annual Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Press Release" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="990">
   <si>
     <t>Some top phrases containing 8 words (without punctuation marks)</t>
   </si>
@@ -2103,6 +2104,897 @@
   </si>
   <si>
     <t>such reports and 2 has been</t>
+  </si>
+  <si>
+    <t>the information was submitted for publication</t>
+  </si>
+  <si>
+    <t>information was submitted for publication through</t>
+  </si>
+  <si>
+    <t>was submitted for publication through the</t>
+  </si>
+  <si>
+    <t>through the agency of the contact</t>
+  </si>
+  <si>
+    <t>to make public pursuant to the</t>
+  </si>
+  <si>
+    <t>publication through the agency of the</t>
+  </si>
+  <si>
+    <t>for publication through the agency of</t>
+  </si>
+  <si>
+    <t>submitted for publication through the agency</t>
+  </si>
+  <si>
+    <t>pursuant to the eu market abuse</t>
+  </si>
+  <si>
+    <t>to the eu market abuse regulation</t>
+  </si>
+  <si>
+    <t>the agency of the contact person</t>
+  </si>
+  <si>
+    <t>public pursuant to the eu market</t>
+  </si>
+  <si>
+    <t>make public pursuant to the eu</t>
+  </si>
+  <si>
+    <t>of the contact person set out</t>
+  </si>
+  <si>
+    <t>agency of the contact person set</t>
+  </si>
+  <si>
+    <t>the contact person set out above</t>
+  </si>
+  <si>
+    <t>is obliged to make public pursuant</t>
+  </si>
+  <si>
+    <t>obliged to make public pursuant to</t>
+  </si>
+  <si>
+    <t>expres2ion biotech holding ab press release</t>
+  </si>
+  <si>
+    <t>biotech holding ab press release 2017</t>
+  </si>
+  <si>
+    <t>robust production of complex proteins for</t>
+  </si>
+  <si>
+    <t>is listed on nasdaq omx stockholm</t>
+  </si>
+  <si>
+    <t>and robust production of complex proteins</t>
+  </si>
+  <si>
+    <t>share is listed on nasdaq omx</t>
+  </si>
+  <si>
+    <t>with company register number 559033 3729</t>
+  </si>
+  <si>
+    <t>expres2ion biotech holding ab with company</t>
+  </si>
+  <si>
+    <t>biotech holding ab with company register</t>
+  </si>
+  <si>
+    <t>subsidiary of expres2ion biotech holding ab</t>
+  </si>
+  <si>
+    <t>ab with company register number 559033</t>
+  </si>
+  <si>
+    <t>holding ab with company register number</t>
+  </si>
+  <si>
+    <t>45 2062 9908 e mail sk@expres2ionbio</t>
+  </si>
+  <si>
+    <t>contact person set out above on</t>
+  </si>
+  <si>
+    <t>telephone 45 2062 9908 e mail</t>
+  </si>
+  <si>
+    <t>has used its patented expres2 platform</t>
+  </si>
+  <si>
+    <t>used its patented expres2 platform to</t>
+  </si>
+  <si>
+    <t>patented expres2 platform to produce more</t>
+  </si>
+  <si>
+    <t>its patented expres2 platform to produce</t>
+  </si>
+  <si>
+    <t>research institutions and biopharmaceutical companies with</t>
+  </si>
+  <si>
+    <t>ceo telephone 45 2062 9908 e</t>
+  </si>
+  <si>
+    <t>with research institutions and biopharmaceutical companies</t>
+  </si>
+  <si>
+    <t>klysner ceo telephone 45 2062 9908</t>
+  </si>
+  <si>
+    <t>steen klysner ceo telephone 45 2062</t>
+  </si>
+  <si>
+    <t>expres2 platform to produce more than</t>
+  </si>
+  <si>
+    <t>tel 46 8 578 646 00</t>
+  </si>
+  <si>
+    <t>a fully owned danish subsidiary of</t>
+  </si>
+  <si>
+    <t>companies with a superior efficiency and</t>
+  </si>
+  <si>
+    <t>stockholm sweden tel 46 8 578</t>
+  </si>
+  <si>
+    <t>cost effective development and robust production</t>
+  </si>
+  <si>
+    <t>93 stockholm sweden tel 46 8</t>
+  </si>
+  <si>
+    <t>effective development and robust production of</t>
+  </si>
+  <si>
+    <t>danish subsidiary of expres2ion biotech holding</t>
+  </si>
+  <si>
+    <t>is a fully owned danish subsidiary</t>
+  </si>
+  <si>
+    <t>with a superior efficiency and success</t>
+  </si>
+  <si>
+    <t>of expres2ion biotech holding ab with</t>
+  </si>
+  <si>
+    <t>103 93 stockholm sweden tel 46</t>
+  </si>
+  <si>
+    <t>proteins for new vaccines and diagnostics</t>
+  </si>
+  <si>
+    <t>of complex proteins for new vaccines</t>
+  </si>
+  <si>
+    <t>owned danish subsidiary of expres2ion biotech</t>
+  </si>
+  <si>
+    <t>a superior efficiency and success rate</t>
+  </si>
+  <si>
+    <t>production of complex proteins for new</t>
+  </si>
+  <si>
+    <t>complex proteins for new vaccines and</t>
+  </si>
+  <si>
+    <t>expres2ion biotechnologies aps is a fully</t>
+  </si>
+  <si>
+    <t>fully owned danish subsidiary of expres2ion</t>
+  </si>
+  <si>
+    <t>sweden tel 46 8 578 646</t>
+  </si>
+  <si>
+    <t>biotechnologies aps is a fully owned</t>
+  </si>
+  <si>
+    <t>development and robust production of complex</t>
+  </si>
+  <si>
+    <t>aps is a fully owned danish</t>
+  </si>
+  <si>
+    <t>appointed as certified adviser for expres2ion</t>
+  </si>
+  <si>
+    <t>as a rescue drug after high</t>
+  </si>
+  <si>
+    <t>and as a rescue drug after</t>
+  </si>
+  <si>
+    <t>in collaborations with research institutions and</t>
+  </si>
+  <si>
+    <t>46 31 701 05 15 e</t>
+  </si>
+  <si>
+    <t>sedermera fondkommission is appointed as certified</t>
+  </si>
+  <si>
+    <t>is appointed as certified adviser for</t>
+  </si>
+  <si>
+    <t>60 fax 46 31 701 05</t>
+  </si>
+  <si>
+    <t>27 gothenburg sweden tel 46 31</t>
+  </si>
+  <si>
+    <t>tel 46 31 60 61 60</t>
+  </si>
+  <si>
+    <t>eye ab första långgatan 28b 413</t>
+  </si>
+  <si>
+    <t>60 61 60 fax 46 31</t>
+  </si>
+  <si>
+    <t>rescue drug after high dose methotrexate</t>
+  </si>
+  <si>
+    <t>31 701 05 15 e mail</t>
+  </si>
+  <si>
+    <t>31 60 61 60 fax 46</t>
+  </si>
+  <si>
+    <t>the share is listed on nasdaq</t>
+  </si>
+  <si>
+    <t>this press release contains information that</t>
+  </si>
+  <si>
+    <t>gothenburg sweden tel 46 31 60</t>
+  </si>
+  <si>
+    <t>46 31 60 61 60 fax</t>
+  </si>
+  <si>
+    <t>sweden tel 46 31 60 61</t>
+  </si>
+  <si>
+    <t>drug after high dose methotrexate treatment</t>
+  </si>
+  <si>
+    <t>28b 413 27 gothenburg sweden tel</t>
+  </si>
+  <si>
+    <t>smart eye ab första långgatan 28b</t>
+  </si>
+  <si>
+    <t>produce more than 200 proteins in</t>
+  </si>
+  <si>
+    <t>platform to produce more than 200</t>
+  </si>
+  <si>
+    <t>fax 46 31 701 05 15</t>
+  </si>
+  <si>
+    <t>ab första långgatan 28b 413 27</t>
+  </si>
+  <si>
+    <t>413 27 gothenburg sweden tel 46</t>
+  </si>
+  <si>
+    <t>701 05 15 e mail info@smarteye</t>
+  </si>
+  <si>
+    <t>långgatan 28b 413 27 gothenburg sweden</t>
+  </si>
+  <si>
+    <t>första långgatan 28b 413 27 gothenburg</t>
+  </si>
+  <si>
+    <t>a rescue drug after high dose</t>
+  </si>
+  <si>
+    <t>fondkommission is appointed as certified adviser</t>
+  </si>
+  <si>
+    <t>61 60 fax 46 31 701</t>
+  </si>
+  <si>
+    <t>to produce more than 200 proteins</t>
+  </si>
+  <si>
+    <t>actual results may differ materially from</t>
+  </si>
+  <si>
+    <t>suitable for all patients irrespective of</t>
+  </si>
+  <si>
+    <t>unique platform technology expres2 enabling cost</t>
+  </si>
+  <si>
+    <t>tgs ability to continue to expand</t>
+  </si>
+  <si>
+    <t>data and tgs ability to acquire</t>
+  </si>
+  <si>
+    <t>fastigheter owns and develops both commercial</t>
+  </si>
+  <si>
+    <t>develops both commercial and residential properties</t>
+  </si>
+  <si>
+    <t>expres2ion expres2ion biotechnologies aps is a</t>
+  </si>
+  <si>
+    <t>the company has used its patented</t>
+  </si>
+  <si>
+    <t>production capabilities of merck kgaa darmstadt</t>
+  </si>
+  <si>
+    <t>to update or alter forward looking</t>
+  </si>
+  <si>
+    <t>a continuous growth in value in</t>
+  </si>
+  <si>
+    <t>residential properties in prioritized growth areas</t>
+  </si>
+  <si>
+    <t>the subsidiary has developed a unique</t>
+  </si>
+  <si>
+    <t>and sought after landlord in our</t>
+  </si>
+  <si>
+    <t>difficult to predict and are based</t>
+  </si>
+  <si>
+    <t>a cyclical industry and principal customers</t>
+  </si>
+  <si>
+    <t>are based upon assumptions as to</t>
+  </si>
+  <si>
+    <t>of historical fact are forward looking</t>
+  </si>
+  <si>
+    <t>expand markets for licensing of data</t>
+  </si>
+  <si>
+    <t>has since 2005 had a continuous</t>
+  </si>
+  <si>
+    <t>both commercial and residential properties in</t>
+  </si>
+  <si>
+    <t>on a cyclical industry and principal</t>
+  </si>
+  <si>
+    <t>founded in 2010 the company has</t>
+  </si>
+  <si>
+    <t>new vaccines and diagnostics for e</t>
+  </si>
+  <si>
+    <t>markets for licensing of data and</t>
+  </si>
+  <si>
+    <t>luleå with its head office in</t>
+  </si>
+  <si>
+    <t>sought after landlord in our market</t>
+  </si>
+  <si>
+    <t>for licensing of data and tgs</t>
+  </si>
+  <si>
+    <t>for new vaccines and diagnostics for</t>
+  </si>
+  <si>
+    <t>with access to the unique patented</t>
+  </si>
+  <si>
+    <t>and principal customers tgs ability to</t>
+  </si>
+  <si>
+    <t>proteins in collaborations with research institutions</t>
+  </si>
+  <si>
+    <t>responsibility or obligation to update or</t>
+  </si>
+  <si>
+    <t>the property portfolio and the share</t>
+  </si>
+  <si>
+    <t>customers tgs ability to continue to</t>
+  </si>
+  <si>
+    <t>learn more about diös on www</t>
+  </si>
+  <si>
+    <t>to the unique patented production process</t>
+  </si>
+  <si>
+    <t>process data products at costs commensurate</t>
+  </si>
+  <si>
+    <t>or obligation to update or alter</t>
+  </si>
+  <si>
+    <t>predict and are based upon assumptions</t>
+  </si>
+  <si>
+    <t>and a lettable area of 1</t>
+  </si>
+  <si>
+    <t>cyclical industry and principal customers tgs</t>
+  </si>
+  <si>
+    <t>technology expres2 enabling cost effective development</t>
+  </si>
+  <si>
+    <t>patented production process and the production</t>
+  </si>
+  <si>
+    <t>those expected or projected in the</t>
+  </si>
+  <si>
+    <t>owns and develops both commercial and</t>
+  </si>
+  <si>
+    <t>expres2 enabling cost effective development and</t>
+  </si>
+  <si>
+    <t>results may differ materially from those</t>
+  </si>
+  <si>
+    <t>– today expres2ion biotech holding ab</t>
+  </si>
+  <si>
+    <t>undertakes no responsibility or obligation to</t>
+  </si>
+  <si>
+    <t>of risks uncertainties and assumptions that</t>
+  </si>
+  <si>
+    <t>on nasdaq omx stockholm mid cap</t>
+  </si>
+  <si>
+    <t>assumptions that are difficult to predict</t>
+  </si>
+  <si>
+    <t>the production capabilities of merck kgaa</t>
+  </si>
+  <si>
+    <t>events that may not prove accurate</t>
+  </si>
+  <si>
+    <t>are subject to a number of</t>
+  </si>
+  <si>
+    <t>vision is to be the most</t>
+  </si>
+  <si>
+    <t>production process and the production capabilities</t>
+  </si>
+  <si>
+    <t>is the key active metabolite of</t>
+  </si>
+  <si>
+    <t>include tgs reliance on a cyclical</t>
+  </si>
+  <si>
+    <t>continuous growth in value in the</t>
+  </si>
+  <si>
+    <t>presentation other than statements of historical</t>
+  </si>
+  <si>
+    <t>and the production capabilities of merck</t>
+  </si>
+  <si>
+    <t>value in the property portfolio and</t>
+  </si>
+  <si>
+    <t>and develops both commercial and residential</t>
+  </si>
+  <si>
+    <t>to be the most active and</t>
+  </si>
+  <si>
+    <t>and residential properties in prioritized growth</t>
+  </si>
+  <si>
+    <t>box 7574 103 93 stockholm sweden</t>
+  </si>
+  <si>
+    <t>and tgs ability to acquire and</t>
+  </si>
+  <si>
+    <t>the company has since 2005 had</t>
+  </si>
+  <si>
+    <t>which are subject to a number</t>
+  </si>
+  <si>
+    <t>continue to expand markets for licensing</t>
+  </si>
+  <si>
+    <t>had a continuous growth in value</t>
+  </si>
+  <si>
+    <t>or projected in the forward looking</t>
+  </si>
+  <si>
+    <t>the key active metabolite of the</t>
+  </si>
+  <si>
+    <t>and process data products at costs</t>
+  </si>
+  <si>
+    <t>upon assumptions as to future events</t>
+  </si>
+  <si>
+    <t>biopharmaceutical companies with a superior efficiency</t>
+  </si>
+  <si>
+    <t>erik penser is certified adviser and</t>
+  </si>
+  <si>
+    <t>future events that may not prove</t>
+  </si>
+  <si>
+    <t>certified adviser and can be reached</t>
+  </si>
+  <si>
+    <t>contact person set out above at</t>
+  </si>
+  <si>
+    <t>in 2010 the company has used</t>
+  </si>
+  <si>
+    <t>growth in value in the property</t>
+  </si>
+  <si>
+    <t>in value in the property portfolio</t>
+  </si>
+  <si>
+    <t>properties and a lettable area of</t>
+  </si>
+  <si>
+    <t>the most active and sought after</t>
+  </si>
+  <si>
+    <t>forward looking statements which are subject</t>
+  </si>
+  <si>
+    <t>to a number of risks uncertainties</t>
+  </si>
+  <si>
+    <t>cancer and as a rescue drug</t>
+  </si>
+  <si>
+    <t>a number of risks uncertainties and</t>
+  </si>
+  <si>
+    <t>than statements of historical fact are</t>
+  </si>
+  <si>
+    <t>collaborations with research institutions and biopharmaceutical</t>
+  </si>
+  <si>
+    <t>process and the production capabilities of</t>
+  </si>
+  <si>
+    <t>properties in prioritized growth areas in</t>
+  </si>
+  <si>
+    <t>statements of historical fact are forward</t>
+  </si>
+  <si>
+    <t>risks uncertainties and assumptions that are</t>
+  </si>
+  <si>
+    <t>company has used its patented expres2</t>
+  </si>
+  <si>
+    <t>statements which are subject to a</t>
+  </si>
+  <si>
+    <t>projected in the forward looking statements</t>
+  </si>
+  <si>
+    <t>key active metabolite of the widely</t>
+  </si>
+  <si>
+    <t>data products at costs commensurate with</t>
+  </si>
+  <si>
+    <t>reliance on a cyclical industry and</t>
+  </si>
+  <si>
+    <t>to acquire and process data products</t>
+  </si>
+  <si>
+    <t>listed on nasdaq omx stockholm mid</t>
+  </si>
+  <si>
+    <t>colorectal cancer and as a rescue</t>
+  </si>
+  <si>
+    <t>all statements in this presentation other</t>
+  </si>
+  <si>
+    <t>principal customers tgs ability to continue</t>
+  </si>
+  <si>
+    <t>to future events that may not</t>
+  </si>
+  <si>
+    <t>has developed a unique platform technology</t>
+  </si>
+  <si>
+    <t>tgs undertakes no responsibility or obligation</t>
+  </si>
+  <si>
+    <t>that are difficult to predict and</t>
+  </si>
+  <si>
+    <t>capabilities of merck kgaa darmstadt germany</t>
+  </si>
+  <si>
+    <t>with its head office in östersund</t>
+  </si>
+  <si>
+    <t>unique patented production process and the</t>
+  </si>
+  <si>
+    <t>to continue to expand markets for</t>
+  </si>
+  <si>
+    <t>to predict and are based upon</t>
+  </si>
+  <si>
+    <t>materially from those expected or projected</t>
+  </si>
+  <si>
+    <t>fact are forward looking statements which</t>
+  </si>
+  <si>
+    <t>uncertainties and assumptions that are difficult</t>
+  </si>
+  <si>
+    <t>access to the unique patented production</t>
+  </si>
+  <si>
+    <t>is certified adviser and can be</t>
+  </si>
+  <si>
+    <t>most active and sought after landlord</t>
+  </si>
+  <si>
+    <t>securities referred to in this announcement</t>
+  </si>
+  <si>
+    <t>metabolite of the widely used folate</t>
+  </si>
+  <si>
+    <t>industry and principal customers tgs ability</t>
+  </si>
+  <si>
+    <t>no responsibility or obligation to update</t>
+  </si>
+  <si>
+    <t>may differ materially from those expected</t>
+  </si>
+  <si>
+    <t>products at costs commensurate with profitability</t>
+  </si>
+  <si>
+    <t>adviser and can be reached at</t>
+  </si>
+  <si>
+    <t>platform technology expres2 enabling cost effective</t>
+  </si>
+  <si>
+    <t>for all patients irrespective of their</t>
+  </si>
+  <si>
+    <t>to luleå with its head office</t>
+  </si>
+  <si>
+    <t>be the most active and sought</t>
+  </si>
+  <si>
+    <t>since 2005 had a continuous growth</t>
+  </si>
+  <si>
+    <t>commercial and residential properties in prioritized</t>
+  </si>
+  <si>
+    <t>active metabolite of the widely used</t>
+  </si>
+  <si>
+    <t>a unique platform technology expres2 enabling</t>
+  </si>
+  <si>
+    <t>expected or projected in the forward</t>
+  </si>
+  <si>
+    <t>these factors include tgs reliance on</t>
+  </si>
+  <si>
+    <t>alter forward looking statements for any</t>
+  </si>
+  <si>
+    <t>2005 had a continuous growth in</t>
+  </si>
+  <si>
+    <t>number of risks uncertainties and assumptions</t>
+  </si>
+  <si>
+    <t>property portfolio and the share is</t>
+  </si>
+  <si>
+    <t>institutions and biopharmaceutical companies with a</t>
+  </si>
+  <si>
+    <t>ability to continue to expand markets</t>
+  </si>
+  <si>
+    <t>ab is obliged to make public</t>
+  </si>
+  <si>
+    <t>developed a unique platform technology expres2</t>
+  </si>
+  <si>
+    <t>prioritized growth areas in northern sweden</t>
+  </si>
+  <si>
+    <t>company has since 2005 had a</t>
+  </si>
+  <si>
+    <t>ability to acquire and process data</t>
+  </si>
+  <si>
+    <t>in the property portfolio and the</t>
+  </si>
+  <si>
+    <t>other than statements of historical fact</t>
+  </si>
+  <si>
+    <t>from those expected or projected in</t>
+  </si>
+  <si>
+    <t>based upon assumptions as to future</t>
+  </si>
+  <si>
+    <t>of data and tgs ability to</t>
+  </si>
+  <si>
+    <t>looking statements which are subject to</t>
+  </si>
+  <si>
+    <t>subject to a number of risks</t>
+  </si>
+  <si>
+    <t>this presentation other than statements of</t>
+  </si>
+  <si>
+    <t>since founded in 2010 the company</t>
+  </si>
+  <si>
+    <t>are forward looking statements which are</t>
+  </si>
+  <si>
+    <t>portfolio and the share is listed</t>
+  </si>
+  <si>
+    <t>as to future events that may</t>
+  </si>
+  <si>
+    <t>differ materially from those expected or</t>
+  </si>
+  <si>
+    <t>2010 the company has used its</t>
+  </si>
+  <si>
+    <t>penser is certified adviser and can</t>
+  </si>
+  <si>
+    <t>is to be the most active</t>
+  </si>
+  <si>
+    <t>tgs reliance on a cyclical industry</t>
+  </si>
+  <si>
+    <t>acquire and process data products at</t>
+  </si>
+  <si>
+    <t>subsidiary has developed a unique platform</t>
+  </si>
+  <si>
+    <t>diös fastigheter owns and develops both</t>
+  </si>
+  <si>
+    <t>and assumptions that are difficult to</t>
+  </si>
+  <si>
+    <t>statements in this presentation other than</t>
+  </si>
+  <si>
+    <t>about expres2ion expres2ion biotechnologies aps is</t>
+  </si>
+  <si>
+    <t>and the share is listed on</t>
+  </si>
+  <si>
+    <t>in prioritized growth areas in northern</t>
+  </si>
+  <si>
+    <t>tgs ability to acquire and process</t>
+  </si>
+  <si>
+    <t>our vision is to be the</t>
+  </si>
+  <si>
+    <t>update or alter forward looking statements</t>
+  </si>
+  <si>
+    <t>and biopharmaceutical companies with a superior</t>
+  </si>
+  <si>
+    <t>licensing of data and tgs ability</t>
+  </si>
+  <si>
+    <t>forward looking statements for any reason</t>
+  </si>
+  <si>
+    <t>factors include tgs reliance on a</t>
+  </si>
+  <si>
+    <t>to expand markets for licensing of</t>
+  </si>
+  <si>
+    <t>in this presentation other than statements</t>
+  </si>
+  <si>
+    <t>and are based upon assumptions as</t>
+  </si>
+  <si>
+    <t>active and sought after landlord in</t>
+  </si>
+  <si>
+    <t>historical fact are forward looking statements</t>
+  </si>
+  <si>
+    <t>are difficult to predict and are</t>
+  </si>
+  <si>
+    <t>obligation to update or alter forward</t>
+  </si>
+  <si>
+    <t>enabling cost effective development and robust</t>
+  </si>
+  <si>
+    <t>or alter forward looking statements for</t>
+  </si>
+  <si>
+    <t>the unique patented production process and</t>
+  </si>
+  <si>
+    <t>assumptions as to future events that</t>
   </si>
 </sst>
 </file>
@@ -2459,7 +3351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+    <sheetView topLeftCell="A161" workbookViewId="0">
       <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
@@ -7773,4 +8665,3299 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C298"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="L276" sqref="L276"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="76" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="C3" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="C4" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="C5" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="C6" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C7" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="C8" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="C9" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="C10" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C11" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="C12" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="C13" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C14" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C15" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C16" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C17" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C18" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="C19" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="C20" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C21" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="C22" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="C23" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="C24" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="C25" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C26" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="C27" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="C28" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="C29" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="C30" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="C31" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="C32" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="C33" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="C34" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="C35" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="C36" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="C37" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="C38" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="C39" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="C40" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C41" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="C42" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="C43" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C44" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C45" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="C46" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="C47" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="C48" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C49" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="C50" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C51" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="C52" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C53" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="C54" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="C55" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="C56" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="C57" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="C58" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="C59" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="C60" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="C61" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="C62" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="C63" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="C64" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="C65" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="C66" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="C67" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="C68" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="C69" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="C70" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="C71" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="C72" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="C73" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="C74" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="C75" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="C76" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="C77" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="C78" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="C79" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="C80" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="C81" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="C82" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="C83" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="C84" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="C85" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="C86" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="C87" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C88" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="C89" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="C90" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="C91" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="C92" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="C93" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="C94" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="C95" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="C96" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="C97" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="C98" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C99" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="C100" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="C101" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="C102" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>2</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="C103" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="C104" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>2</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="C105" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="C106" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>2</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="C107" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="C108" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="C109" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>2</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="C110" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="C111" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>2</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="C112" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>2</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="C113" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="C114" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>2</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="C115" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="C116" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>2</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="C117" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>2</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="C118" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>2</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="C119" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>2</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="C120" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>2</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="C121" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>2</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="C122" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>2</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="C123" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>2</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="C124" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>2</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="C125" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>2</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="C126" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>2</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="C127" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>2</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="C128" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>2</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="C129" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>2</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="C130" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>2</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="C131" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>2</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="C132" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>2</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="C133" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>2</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="C134" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>2</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="C135" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>2</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="C136" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>2</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C137" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>2</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="C138" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>2</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="C139" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>2</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C140" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>2</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="C141" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>2</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="C142" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>2</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="C143" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>2</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="C144" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>2</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="C145" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>2</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="C146" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>2</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="C147" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>2</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="C148" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>2</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="C149" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>2</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="C150" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>2</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="C151" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>2</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="C152" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>2</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="C153" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>2</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="C154" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>2</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="C155" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>2</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="C156" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>2</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="C157" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>2</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="C158" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>2</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="C159" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>2</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="C160" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>2</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="C161" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>2</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="C162" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>2</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="C163" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>2</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="C164" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>2</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="C165" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>2</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="C166" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>2</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="C167" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>2</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="C168" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>2</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="C169" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>2</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="C170" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>2</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="C171" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>2</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="C172" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>2</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="C173" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>2</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="C174" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>2</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C175" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>2</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="C176" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>2</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="C177" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>2</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="C178" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>2</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="C179" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>2</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="C180" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>2</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="C181" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>2</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="C182" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>2</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="C183" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>2</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="C184" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>2</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="C185" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>2</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="C186" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>2</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="C187" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>2</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="C188" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>2</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="C189" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>2</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="C190" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>2</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="C191" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>2</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="C192" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>2</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="C193" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>2</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="C194" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>2</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="C195" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>2</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="C196" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>2</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="C197" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>2</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="C198" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>2</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="C199" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>2</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="C200" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>2</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="C201" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>2</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="C202" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>2</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="C203" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>2</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="C204" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>2</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="C205" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>2</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="C206" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>2</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="C207" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>2</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="C208" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>2</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="C209" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>2</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="C210" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>2</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="C211" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>2</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="C212" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>2</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="C213" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>2</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="C214" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>2</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="C215" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>2</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="C216" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>2</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="C217" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>2</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="C218" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>2</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="C219" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>2</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="C220" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>2</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="C221" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>2</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="C222" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>2</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="C223" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>2</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="C224" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>2</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="C225" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>2</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="C226" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>2</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="C227" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>2</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="C228" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>2</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="C229" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>2</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="C230" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>2</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="C231" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>2</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="C232" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>2</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="C233" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>2</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="C234" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>2</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="C235" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>2</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="C236" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>2</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="C237" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>2</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="C238" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>2</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="C239" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>2</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="C240" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>2</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="C241" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>2</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="C242" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>2</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="C243" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>2</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="C244" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>2</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="C245" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>2</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="C246" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>2</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="C247" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>2</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="C248" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>2</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="C249" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>2</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="C250" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>2</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="C251" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>2</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="C252" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>2</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="C253" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>2</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="C254" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>2</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="C255" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>2</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="C256" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>2</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="C257" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>2</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="C258" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>2</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="C259" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>2</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="C260" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>2</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="C261" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>2</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="C262" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>2</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="C263" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>2</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="C264" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>2</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="C265" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>2</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>957</v>
+      </c>
+      <c r="C266" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>2</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="C267" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>2</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="C268" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>2</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="C269" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>2</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="C270" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>2</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="C271" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>2</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="C272" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>2</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="C273" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>2</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="C274" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>2</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="C275" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>2</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="C276" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>2</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="C277" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>2</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="C278" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>2</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="C279" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>2</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="C280" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>2</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="C281" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>2</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="C282" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>2</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="C283" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>2</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="C284" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>2</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="C285" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>2</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="C286" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>2</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="C287" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>2</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="C288" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>2</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="C289" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>2</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="C290" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>2</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="C291" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>2</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="C292" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>2</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="C293" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>2</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C294" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>2</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="C295" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>2</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="C296" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>2</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="C297" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>2</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="C298" s="3">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>